<commit_message>
Added proper error logging and refactor cms_case_loaders.
Added error logs to charges_grids.


Added logging to main function.


Added log to main to track which host loads application.


Updated logger.


Logging updated to warning for attribute errors.


Added comment for load_window.


Cleaning up cms_case_loaders


Fixed test_databases as a result of updating dbs in test.


Fixed all tests caused by DB change.


Finished flake8, pylint and mypy for cms_case_loaders.
</commit_message>
<xml_diff>
--- a/db/Pleas.xlsx
+++ b/db/Pleas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B3456E-67C7-465E-9337-C27F102658CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F8499E-2707-4708-A415-33F25A89AEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MuniEntryPleas" sheetId="1" r:id="rId1"/>
@@ -184,9 +184,6 @@
     <t>21CRB01597-A</t>
   </si>
   <si>
-    <t>ANSLEY</t>
-  </si>
-  <si>
     <t>JACOB</t>
   </si>
   <si>
@@ -401,6 +398,9 @@
   </si>
   <si>
     <t>4511.13C</t>
+  </si>
+  <si>
+    <t>O'Reilly</t>
   </si>
 </sst>
 </file>
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1233,16 +1233,16 @@
         <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>40</v>
@@ -1252,7 +1252,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>26</v>
@@ -1261,22 +1261,22 @@
     </row>
     <row r="11" spans="1:12" ht="25.5">
       <c r="A11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>36</v>
@@ -1288,7 +1288,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>26</v>
@@ -1297,22 +1297,22 @@
     </row>
     <row r="12" spans="1:12" ht="38.25">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>36</v>
@@ -1324,7 +1324,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>26</v>
@@ -1333,16 +1333,16 @@
     </row>
     <row r="13" spans="1:12" ht="38.25">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>38</v>
@@ -1360,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>26</v>
@@ -1369,16 +1369,16 @@
     </row>
     <row r="14" spans="1:12" ht="38.25">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>45</v>
@@ -1396,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>26</v>
@@ -1405,16 +1405,16 @@
     </row>
     <row r="15" spans="1:12" ht="25.5">
       <c r="A15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>27</v>
@@ -1426,103 +1426,103 @@
         <v>29</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I15" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="38.25">
       <c r="A16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="38.25">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="38.25">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>38</v>
@@ -1534,31 +1534,31 @@
         <v>40</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I18" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="25.5">
       <c r="A19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>27</v>
@@ -1570,103 +1570,103 @@
         <v>29</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I19" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="51">
       <c r="A20" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I20" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="25.5">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I21" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="25.5">
       <c r="A22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>27</v>
@@ -1678,11 +1678,11 @@
         <v>29</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>26</v>
@@ -1691,32 +1691,32 @@
     </row>
     <row r="23" spans="1:12" ht="38.25">
       <c r="A23" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="E23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>26</v>
@@ -1725,94 +1725,94 @@
     </row>
     <row r="24" spans="1:12" ht="51">
       <c r="A24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="E24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I24" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="25.5">
       <c r="A25" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="F25" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I25" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="25.5">
       <c r="A26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
@@ -1827,16 +1827,16 @@
     </row>
     <row r="27" spans="1:12" ht="25.5">
       <c r="A27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>27</v>
@@ -1848,43 +1848,43 @@
         <v>29</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I27" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" ht="38.25">
       <c r="A28" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I28" s="2" t="b">
         <v>1</v>
@@ -1895,28 +1895,28 @@
     </row>
     <row r="29" spans="1:12" ht="38.25">
       <c r="A29" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I29" s="2" t="b">
         <v>1</v>

</xml_diff>